<commit_message>
update in table data
</commit_message>
<xml_diff>
--- a/public/covid_AL_spreadsheet.xlsx
+++ b/public/covid_AL_spreadsheet.xlsx
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="442" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="446" uniqueCount="10">
   <si>
     <t xml:space="preserve">region</t>
   </si>
@@ -60,7 +60,7 @@
     <numFmt numFmtId="164" formatCode="General"/>
     <numFmt numFmtId="165" formatCode="D/M/YYYY"/>
   </numFmts>
-  <fonts count="5">
+  <fonts count="7">
     <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
@@ -87,6 +87,20 @@
       <sz val="8"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
+      <family val="0"/>
+      <charset val="1"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color rgb="FF000000"/>
+      <name val="Arial"/>
       <family val="0"/>
       <charset val="1"/>
     </font>
@@ -133,7 +147,7 @@
     <xf numFmtId="42" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
     <xf numFmtId="9" fontId="1" fillId="0" borderId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false"/>
   </cellStyleXfs>
-  <cellXfs count="6">
+  <cellXfs count="7">
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="false" applyBorder="false" applyAlignment="false" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
@@ -142,7 +156,7 @@
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
-    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="false" applyProtection="false">
+    <xf numFmtId="164" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
@@ -156,6 +170,10 @@
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
       <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="true" indent="0" shrinkToFit="false"/>
+      <protection locked="true" hidden="false"/>
+    </xf>
+    <xf numFmtId="164" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="true" applyBorder="false" applyAlignment="true" applyProtection="false">
+      <alignment horizontal="right" vertical="bottom" textRotation="0" wrapText="false" indent="0" shrinkToFit="false"/>
       <protection locked="true" hidden="false"/>
     </xf>
   </cellXfs>
@@ -175,21 +193,18 @@
   <sheetPr filterMode="false">
     <pageSetUpPr fitToPage="false"/>
   </sheetPr>
-  <dimension ref="A1:I218"/>
+  <dimension ref="A1:I1048576"/>
   <sheetViews>
     <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="100" zoomScaleNormal="100" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="H3" activeCellId="0" sqref="H3"/>
+      <selection pane="topLeft" activeCell="I14" activeCellId="0" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="1" style="0" width="14.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="0" width="16.3"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="0" width="16.99"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="8" style="0" width="14.43"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1025" min="1" style="0" width="14.43"/>
   </cols>
   <sheetData>
-    <row r="1" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+    <row r="1" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -211,7 +226,7 @@
       <c r="G1" s="1" t="s">
         <v>6</v>
       </c>
-      <c r="I1" s="2" t="s">
+      <c r="H1" s="2" t="s">
         <v>7</v>
       </c>
     </row>
@@ -237,9 +252,10 @@
       <c r="G2" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="I2" s="5" t="n">
-        <v>84720</v>
-      </c>
+      <c r="H2" s="5" t="n">
+        <v>87504</v>
+      </c>
+      <c r="I2" s="6"/>
     </row>
     <row r="3" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="1" t="s">
@@ -263,9 +279,10 @@
       <c r="G3" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="I3" s="5" t="n">
-        <v>85008</v>
-      </c>
+      <c r="H3" s="5" t="n">
+        <v>87750</v>
+      </c>
+      <c r="I3" s="6"/>
     </row>
     <row r="4" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1" t="s">
@@ -289,9 +306,10 @@
       <c r="G4" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="I4" s="5" t="n">
-        <v>85559</v>
-      </c>
+      <c r="H4" s="5" t="n">
+        <v>87928</v>
+      </c>
+      <c r="I4" s="6"/>
     </row>
     <row r="5" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
@@ -315,9 +333,10 @@
       <c r="G5" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="I5" s="5" t="n">
-        <v>85753</v>
-      </c>
+      <c r="H5" s="5" t="n">
+        <v>88098</v>
+      </c>
+      <c r="I5" s="6"/>
     </row>
     <row r="6" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="1" t="s">
@@ -341,9 +360,10 @@
       <c r="G6" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="I6" s="5" t="n">
-        <v>85937</v>
-      </c>
+      <c r="H6" s="5" t="n">
+        <v>88135</v>
+      </c>
+      <c r="I6" s="6"/>
     </row>
     <row r="7" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="1" t="s">
@@ -367,9 +387,10 @@
       <c r="G7" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="I7" s="5" t="n">
-        <v>86124</v>
-      </c>
+      <c r="H7" s="5" t="n">
+        <v>88283</v>
+      </c>
+      <c r="I7" s="6"/>
     </row>
     <row r="8" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="1" t="s">
@@ -393,11 +414,12 @@
       <c r="G8" s="4" t="n">
         <v>0</v>
       </c>
-      <c r="I8" s="5" t="n">
-        <v>86294</v>
-      </c>
-    </row>
-    <row r="9" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H8" s="5" t="n">
+        <v>88426</v>
+      </c>
+      <c r="I8" s="6"/>
+    </row>
+    <row r="9" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="1" t="s">
         <v>8</v>
       </c>
@@ -419,8 +441,12 @@
       <c r="G9" s="4" t="n">
         <v>0</v>
       </c>
-    </row>
-    <row r="10" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H9" s="5" t="n">
+        <v>88538</v>
+      </c>
+      <c r="I9" s="6"/>
+    </row>
+    <row r="10" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="1" t="s">
         <v>8</v>
       </c>
@@ -442,8 +468,12 @@
       <c r="G10" s="4" t="n">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H10" s="5" t="n">
+        <v>88653</v>
+      </c>
+      <c r="I10" s="6"/>
+    </row>
+    <row r="11" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="1" t="s">
         <v>8</v>
       </c>
@@ -465,8 +495,12 @@
       <c r="G11" s="4" t="n">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H11" s="5" t="n">
+        <v>88790</v>
+      </c>
+      <c r="I11" s="6"/>
+    </row>
+    <row r="12" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="1" t="s">
         <v>8</v>
       </c>
@@ -488,8 +522,12 @@
       <c r="G12" s="4" t="n">
         <v>0</v>
       </c>
-    </row>
-    <row r="13" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H12" s="5" t="n">
+        <v>88826</v>
+      </c>
+      <c r="I12" s="6"/>
+    </row>
+    <row r="13" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="1" t="s">
         <v>8</v>
       </c>
@@ -511,8 +549,12 @@
       <c r="G13" s="4" t="n">
         <v>0</v>
       </c>
-    </row>
-    <row r="14" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H13" s="5" t="n">
+        <v>88880</v>
+      </c>
+      <c r="I13" s="6"/>
+    </row>
+    <row r="14" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="1" t="s">
         <v>8</v>
       </c>
@@ -534,8 +576,12 @@
       <c r="G14" s="4" t="n">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H14" s="5" t="n">
+        <v>88954</v>
+      </c>
+      <c r="I14" s="6"/>
+    </row>
+    <row r="15" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A15" s="1" t="s">
         <v>8</v>
       </c>
@@ -557,8 +603,12 @@
       <c r="G15" s="4" t="n">
         <v>0</v>
       </c>
-    </row>
-    <row r="16" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H15" s="5" t="n">
+        <v>89082</v>
+      </c>
+      <c r="I15" s="6"/>
+    </row>
+    <row r="16" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="1" t="s">
         <v>8</v>
       </c>
@@ -580,8 +630,12 @@
       <c r="G16" s="4" t="n">
         <v>0</v>
       </c>
-    </row>
-    <row r="17" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H16" s="5" t="n">
+        <v>89192</v>
+      </c>
+      <c r="I16" s="6"/>
+    </row>
+    <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A17" s="1" t="s">
         <v>8</v>
       </c>
@@ -603,8 +657,12 @@
       <c r="G17" s="4" t="n">
         <v>0</v>
       </c>
-    </row>
-    <row r="18" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H17" s="5" t="n">
+        <v>89278</v>
+      </c>
+      <c r="I17" s="6"/>
+    </row>
+    <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A18" s="1" t="s">
         <v>8</v>
       </c>
@@ -626,8 +684,12 @@
       <c r="G18" s="4" t="n">
         <v>0</v>
       </c>
-    </row>
-    <row r="19" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H18" s="5" t="n">
+        <v>89365</v>
+      </c>
+      <c r="I18" s="6"/>
+    </row>
+    <row r="19" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A19" s="1" t="s">
         <v>8</v>
       </c>
@@ -649,8 +711,12 @@
       <c r="G19" s="4" t="n">
         <v>0</v>
       </c>
-    </row>
-    <row r="20" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H19" s="5" t="n">
+        <v>89493</v>
+      </c>
+      <c r="I19" s="6"/>
+    </row>
+    <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A20" s="1" t="s">
         <v>8</v>
       </c>
@@ -672,8 +738,12 @@
       <c r="G20" s="4" t="n">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H20" s="5" t="n">
+        <v>89528</v>
+      </c>
+      <c r="I20" s="6"/>
+    </row>
+    <row r="21" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="1" t="s">
         <v>8</v>
       </c>
@@ -695,8 +765,12 @@
       <c r="G21" s="4" t="n">
         <v>0</v>
       </c>
-    </row>
-    <row r="22" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H21" s="5" t="n">
+        <v>89644</v>
+      </c>
+      <c r="I21" s="6"/>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="1" t="s">
         <v>8</v>
       </c>
@@ -718,8 +792,9 @@
       <c r="G22" s="4" t="n">
         <v>0</v>
       </c>
-    </row>
-    <row r="23" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H22" s="5"/>
+    </row>
+    <row r="23" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="1" t="s">
         <v>8</v>
       </c>
@@ -741,8 +816,9 @@
       <c r="G23" s="4" t="n">
         <v>0</v>
       </c>
-    </row>
-    <row r="24" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H23" s="5"/>
+    </row>
+    <row r="24" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
         <v>8</v>
       </c>
@@ -764,8 +840,9 @@
       <c r="G24" s="4" t="n">
         <v>0</v>
       </c>
-    </row>
-    <row r="25" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H24" s="5"/>
+    </row>
+    <row r="25" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
         <v>8</v>
       </c>
@@ -787,8 +864,9 @@
       <c r="G25" s="4" t="n">
         <v>0</v>
       </c>
-    </row>
-    <row r="26" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H25" s="5"/>
+    </row>
+    <row r="26" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
         <v>8</v>
       </c>
@@ -810,8 +888,9 @@
       <c r="G26" s="4" t="n">
         <v>0</v>
       </c>
-    </row>
-    <row r="27" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H26" s="5"/>
+    </row>
+    <row r="27" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
         <v>8</v>
       </c>
@@ -833,8 +912,9 @@
       <c r="G27" s="4" t="n">
         <v>0</v>
       </c>
-    </row>
-    <row r="28" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H27" s="5"/>
+    </row>
+    <row r="28" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
         <v>8</v>
       </c>
@@ -856,8 +936,9 @@
       <c r="G28" s="4" t="n">
         <v>0</v>
       </c>
-    </row>
-    <row r="29" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="H28" s="5"/>
+    </row>
+    <row r="29" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
         <v>8</v>
       </c>
@@ -879,6 +960,7 @@
       <c r="G29" s="4" t="n">
         <v>0</v>
       </c>
+      <c r="H29" s="5"/>
     </row>
     <row r="30" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
@@ -5227,6 +5309,53 @@
         <v>2062</v>
       </c>
     </row>
+    <row r="219" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A219" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B219" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C219" s="3" t="n">
+        <v>44103</v>
+      </c>
+      <c r="D219" s="6" t="n">
+        <v>156</v>
+      </c>
+      <c r="E219" s="6" t="n">
+        <v>5</v>
+      </c>
+      <c r="F219" s="6" t="n">
+        <v>86549</v>
+      </c>
+      <c r="G219" s="6" t="n">
+        <v>2067</v>
+      </c>
+    </row>
+    <row r="220" customFormat="false" ht="15.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="A220" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B220" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C220" s="3" t="n">
+        <v>44104</v>
+      </c>
+      <c r="D220" s="6" t="n">
+        <v>330</v>
+      </c>
+      <c r="E220" s="6" t="n">
+        <v>5</v>
+      </c>
+      <c r="F220" s="6" t="n">
+        <v>86879</v>
+      </c>
+      <c r="G220" s="6" t="n">
+        <v>2072</v>
+      </c>
+    </row>
+    <row r="1048576" customFormat="false" ht="15.75" hidden="false" customHeight="true" outlineLevel="0" collapsed="false"/>
   </sheetData>
   <printOptions headings="false" gridLines="false" gridLinesSet="true" horizontalCentered="false" verticalCentered="false"/>
   <pageMargins left="0.747916666666667" right="0.747916666666667" top="0.984027777777778" bottom="0.984027777777778" header="0.511805555555555" footer="0.511805555555555"/>

</xml_diff>